<commit_message>
Actualizar datos agregados de Covid-19 y SARS
</commit_message>
<xml_diff>
--- a/01_datos/covid19_sars/datos_coronavirus.xlsx
+++ b/01_datos/covid19_sars/datos_coronavirus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/segasi/Google Drive/R/04 medios/adn40/2020/bi_covid19/01_datos/covid19_sars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F625CB-0D08-A840-A245-38733ABCA84B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47D9000-1F83-3444-B722-FB3B77F10A60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9080" yWindow="1100" windowWidth="23940" windowHeight="18820" xr2:uid="{4A67F9D4-A6BB-044A-96D6-BB85D48776F5}"/>
+    <workbookView xWindow="14900" yWindow="460" windowWidth="23940" windowHeight="18820" xr2:uid="{4A67F9D4-A6BB-044A-96D6-BB85D48776F5}"/>
   </bookViews>
   <sheets>
     <sheet name="novel_coronavirus" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="194">
   <si>
     <t>casos_totales</t>
   </si>
@@ -618,13 +618,16 @@
   </si>
   <si>
     <t>https://www.cancilleria.gob.ec/ecuador-suspende-vuelos-de-pasajeros-desde-el-exterior-hasta-el-5-de-abril/; https://www.cancilleria.gob.ec/cuarentena-covid-19-aislamiento-preventivo-obligatorio-apo/</t>
+  </si>
+  <si>
+    <t>https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html#/bda7594740fd40299423467b48e9ecf8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -686,6 +689,12 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1038,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B324DF51-79BB-4E43-8C5F-28610EC97764}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="144" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="144" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2213,7 +2222,217 @@
         <v>15</v>
       </c>
     </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B71">
+        <v>467594</v>
+      </c>
+      <c r="C71">
+        <v>21181</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="1">
+        <v>43916</v>
+      </c>
+      <c r="B72">
+        <v>529591</v>
+      </c>
+      <c r="C72">
+        <v>23970</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B73">
+        <v>593291</v>
+      </c>
+      <c r="C73">
+        <v>27198</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="1">
+        <v>43918</v>
+      </c>
+      <c r="B74">
+        <v>660706</v>
+      </c>
+      <c r="C74">
+        <v>30652</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B75">
+        <v>720117</v>
+      </c>
+      <c r="C75">
+        <v>33925</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B76">
+        <v>782365</v>
+      </c>
+      <c r="C76">
+        <v>37582</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="1">
+        <v>43921</v>
+      </c>
+      <c r="B77">
+        <v>857487</v>
+      </c>
+      <c r="C77">
+        <v>42107</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B78">
+        <v>932605</v>
+      </c>
+      <c r="C78">
+        <v>46809</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B79">
+        <v>1013157</v>
+      </c>
+      <c r="C79">
+        <v>52983</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B80">
+        <v>1095917</v>
+      </c>
+      <c r="C80">
+        <v>58787</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="1">
+        <v>43925</v>
+      </c>
+      <c r="B81">
+        <v>1197405</v>
+      </c>
+      <c r="C81">
+        <v>64606</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1">
+        <v>43926</v>
+      </c>
+      <c r="B82">
+        <v>1272115</v>
+      </c>
+      <c r="C82">
+        <v>69374</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="1">
+        <v>43927</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{1E63184E-DB9D-3843-8E7C-A54241A55C80}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{6EB3DA0E-7484-2742-979B-C356997FE1EB}"/>
@@ -2280,6 +2499,18 @@
     <hyperlink ref="E68" r:id="rId63" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{CDFBCCE3-8C13-A843-B630-DEE84142CC18}"/>
     <hyperlink ref="E69" r:id="rId64" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{A5CED9DD-8D6E-8844-941C-BCD687200566}"/>
     <hyperlink ref="E70" r:id="rId65" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{D7642484-C042-C84F-9A21-8DBBEF6E1B72}"/>
+    <hyperlink ref="E71" r:id="rId66" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{8FAE618C-0F1E-394F-9829-6FBCD950BFEE}"/>
+    <hyperlink ref="E72" r:id="rId67" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{0DB1E8A6-617A-1044-83A9-7513B3BB2E5F}"/>
+    <hyperlink ref="E73" r:id="rId68" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{95A3A070-C324-3948-9D1B-1870DF294110}"/>
+    <hyperlink ref="E74" r:id="rId69" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{9F27F680-9894-3440-87F2-57D2D6964E45}"/>
+    <hyperlink ref="E75" r:id="rId70" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{D014D4A4-E5C0-BA42-8CBD-67EC04E60D7D}"/>
+    <hyperlink ref="E76" r:id="rId71" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{2585DD5D-CF8A-2A41-A251-535AA80B8427}"/>
+    <hyperlink ref="E77" r:id="rId72" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{D2B5586B-311D-3846-8543-89A127E9B6A1}"/>
+    <hyperlink ref="E78" r:id="rId73" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{8932B44D-BD22-EB40-B283-FD87B7723A1C}"/>
+    <hyperlink ref="E79" r:id="rId74" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{13BD02E1-3A0E-0D4D-B0B4-9AE3DF3BD306}"/>
+    <hyperlink ref="E80" r:id="rId75" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{D0B20796-DE83-804F-A28F-E1B21063EDCA}"/>
+    <hyperlink ref="E81" r:id="rId76" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{CC3A25B8-8F19-5142-89FA-0CD1A94438AA}"/>
+    <hyperlink ref="E82" r:id="rId77" location="/bda7594740fd40299423467b48e9ecf6" display="https://gisanddata.maps.arcgis.com/apps/opsdashboard/index.html - /bda7594740fd40299423467b48e9ecf6" xr:uid="{1C18269D-44C5-7F44-AEC5-96B278A0002B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3734,8 +3965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26AD6D0-47E5-2440-BC53-655C4DEC0454}">
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>

</xml_diff>